<commit_message>
update from SVN to preserve
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
+++ b/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationAssignment\3. Delivery\02_HeThongSoTayLienLacDienTu\trunk\source\E2PortalProject-master\src\main\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationAssignment\3. Delivery\02_HeThongSoTayLienLacDienTu\trunk\source\E2PortalProject-master\src\main\resources\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD23331-9F4A-4E4F-8527-379BCB81B464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D4476-435D-4F8A-AD22-F301BE9D49BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3075" windowWidth="18930" windowHeight="7995" xr2:uid="{71F0CB4C-2A2F-4E55-85BB-AFFA7FB33296}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{71F0CB4C-2A2F-4E55-85BB-AFFA7FB33296}"/>
   </bookViews>
   <sheets>
     <sheet name="420300048763" sheetId="1" r:id="rId1"/>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A83E66-074B-4CF2-BB07-16B874E22AE9}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -795,10 +795,11 @@
     <col min="2" max="2" width="23" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.28515625" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
preserve from SVN to backup
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
+++ b/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationAssignment\3. Delivery\02_HeThongSoTayLienLacDienTu\trunk\source\E2PortalProject-master\src\main\resources\static\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationAssignment\3. Delivery\02_HeThongSoTayLienLacDienTu\trunk\source\E2PortalProject\src\main\resources\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D4476-435D-4F8A-AD22-F301BE9D49BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3AAF97-87B0-4267-8532-1CCD5ED8845E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{71F0CB4C-2A2F-4E55-85BB-AFFA7FB33296}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
   <si>
     <t>Giữa kỳ</t>
   </si>
@@ -301,18 +301,32 @@
   </si>
   <si>
     <t>GDR</t>
+  </si>
+  <si>
+    <t>Khoa</t>
+  </si>
+  <si>
+    <t>CNTT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -447,27 +461,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A83E66-074B-4CF2-BB07-16B874E22AE9}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -837,7 +853,9 @@
       <c r="J1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="14"/>
+      <c r="K1" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -871,7 +889,9 @@
       <c r="J2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Grading Result Imported only now show with moduleclass
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
+++ b/src/main/resources/static/excels/DANHSACHDIEM_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GraduationAssignment\3. Delivery\02_HeThongSoTayLienLacDienTu\trunk\source\E2PortalProject\src\main\resources\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3AAF97-87B0-4267-8532-1CCD5ED8845E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BBF2F4-F71C-4486-814D-5836883FA1A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{71F0CB4C-2A2F-4E55-85BB-AFFA7FB33296}"/>
   </bookViews>
@@ -291,9 +291,6 @@
     <t>Tên giảng viên</t>
   </si>
   <si>
-    <t>Công nghệ mới</t>
-  </si>
-  <si>
     <t>HK 2 2016-2020</t>
   </si>
   <si>
@@ -307,18 +304,29 @@
   </si>
   <si>
     <t>CNTT</t>
+  </si>
+  <si>
+    <t>Công nghệ cũ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,29 +469,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,7 +811,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -854,16 +863,16 @@
         <v>85</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
-        <v>420300048764</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>86</v>
+        <v>420300048664</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="C2" s="9">
         <v>4</v>
@@ -881,22 +890,22 @@
         <v>44038</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I2" s="13">
         <v>123456</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L2" s="15"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>